<commit_message>
Scrape papers from jmlr
</commit_message>
<xml_diff>
--- a/skills/Other Skills.xlsx
+++ b/skills/Other Skills.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kongbinxuan/Desktop/skills-onthology-project/skills/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kongbinxuan/Desktop/python-web-scraper/skills/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22062155-82AF-B445-9CD0-F3CAE5440D70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102ED3FC-A3E1-7842-8E54-F56C9CF295FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13720" yWindow="460" windowWidth="15080" windowHeight="16180" activeTab="1" xr2:uid="{273D56F0-60F4-7D4D-B74A-F5CA8C152A80}"/>
+    <workbookView xWindow="13720" yWindow="500" windowWidth="15080" windowHeight="16100" xr2:uid="{273D56F0-60F4-7D4D-B74A-F5CA8C152A80}"/>
   </bookViews>
   <sheets>
     <sheet name="Redundant" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="219">
   <si>
     <t>Skill</t>
   </si>
@@ -689,6 +689,9 @@
   </si>
   <si>
     <t>Microsoft Publisher</t>
+  </si>
+  <si>
+    <t>TestNG</t>
   </si>
 </sst>
 </file>
@@ -799,8 +802,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FCFD10E1-5310-7346-AC41-980E95A43B73}" name="Table1" displayName="Table1" ref="A1:A43" totalsRowShown="0">
-  <autoFilter ref="A1:A43" xr:uid="{70E2AE85-8354-604E-A8F5-BA1E0909D1D5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FCFD10E1-5310-7346-AC41-980E95A43B73}" name="Table1" displayName="Table1" ref="A1:A44" totalsRowShown="0">
+  <autoFilter ref="A1:A44" xr:uid="{70E2AE85-8354-604E-A8F5-BA1E0909D1D5}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A43">
     <sortCondition ref="A1:A43"/>
   </sortState>
@@ -1122,10 +1125,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E914D5-27CD-7E41-A3B3-3B307D4A30A6}">
-  <dimension ref="A1:A43"/>
+  <dimension ref="A1:A44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1346,6 +1349,11 @@
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -1360,7 +1368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A8B7B5-E1C1-554A-873B-35A5AF2000A8}">
   <dimension ref="A1:B94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+    <sheetView topLeftCell="A110" workbookViewId="0">
       <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>

</xml_diff>